<commit_message>
reading text exercise completed
</commit_message>
<xml_diff>
--- a/public/docs/Reading_texts.xlsx
+++ b/public/docs/Reading_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B842EA-0A40-4636-903F-3CDD199BA116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748903A9-EC05-4587-ACFE-2AC868C44CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B3869C71-3D6A-4C15-B9E8-2F98229CC412}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
-    <t>TEXT 1 Liam and Emma love to explore the world. One day, they found an old map in their grandfather\’s attic. “We need to find out where this leads!” Emma said excitedly. The information on the map was faded, but it showed a big red "X" in the middle of a forest. "How much treasure do you think is buried there?" Liam asked. \n \n "Let\'s take the map and go on an adventure!" Emma said. The two of them packed their bags and set off. They didn\'t know what they would find, but they knew one thing for sure—they want an adventure over anything else! The two of them packed their bags and set off. They didn\'t know what they would find, but they knew one thing for sure—they want an adventure over anything else!',</t>
-  </si>
-  <si>
     <t>\n \n</t>
   </si>
   <si>
@@ -144,6 +141,18 @@
   </si>
   <si>
     <t>//TEXT 30</t>
+  </si>
+  <si>
+    <t>Many people need water every day to live.
+Some places don’t have enough, so they must find new ways to get it.
+There are different tools that people can use to clean water.
+Most of these tools are good, but some are only used in big cities.
+Other tools are also made for small towns.
+All of this work is about helping people stay healthy.
+Even kids can learn what to do in hard times.
+It has been a long time, but things are just starting to improve.
+People like to see progress, because it gives them hope.
+They want to make a film to show how people used their ideas to go through such challenges.',</t>
   </si>
 </sst>
 </file>
@@ -539,7 +548,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -549,318 +558,318 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="150" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="165" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="15" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reading texts completed for 10 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Reading_texts.xlsx
+++ b/public/docs/Reading_texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5284CAA6-B8E4-4DEA-9C99-248B903CC442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63407941-1CA8-4831-983A-206323A3B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B3869C71-3D6A-4C15-B9E8-2F98229CC412}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>\n \n</t>
   </si>
@@ -147,6 +147,16 @@
   </si>
   <si>
     <t>`I like history. People often talk about it. Then, people did not have maps. They would travel and try to find new places. They wanted to find gold and make money. The world was big to them. \n \nWe know many things now. Well, some things are still a mystery. Now, we have a map of the whole world. It is easy to find places today.`,</t>
+  </si>
+  <si>
+    <t>`A SIMPLE DAY\n \nA few birds sang. I think they were happy. The sky was free of clouds. It was warm too. After breakfast, I used my computer. It was the best part of the day. Life felt calm and slow. I smiled all morning. The day was quiet. It was a good day.`,</t>
+  </si>
+  <si>
+    <t>`The best part was over. \n \nShe walked across the field. \n \nHelp was not available right away. \n \nHe sat down to wait. \n \nA local man passed by. \n \nSomething felt strange. \n \nIn general, things were quiet. \n \nThe process took time. \n \nThe heat was rising fast. \n \nThey had enough for now.`,</t>
+  </si>
+  <si>
+    <t>`A Quiet Morning\n
+She woke up early. Her job didn’t start for hours. At home, she liked to read with music playing. The food was simple but warm. She never skipped breakfast. It was really peaceful. She wasn\’t certain what the day would be like. But she hoped it would include something kind. To her, that was enough. She smiled and felt ready.`,</t>
   </si>
 </sst>
 </file>
@@ -541,8 +551,8 @@
   <dimension ref="B1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -591,9 +601,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" x14ac:dyDescent="0.3">
@@ -601,9 +611,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.3">
@@ -611,9 +621,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="105.6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.3">

</xml_diff>